<commit_message>
Report parts are combined.
</commit_message>
<xml_diff>
--- a/FinalReport/Bill of Materials.xlsx
+++ b/FinalReport/Bill of Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EE464\KOM-19\FinalReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{364473E5-DC20-4697-AEC8-A5A883EE3DAB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCF32DF-A41D-4274-AF33-8E4C8C7EA2D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0D794A8B-9F34-4898-B56B-37206F6CAB8F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="101">
   <si>
     <t>Comment</t>
   </si>
@@ -105,12 +105,6 @@
     <t>TST20U100CC0G</t>
   </si>
   <si>
-    <t>8TQ080</t>
-  </si>
-  <si>
-    <t>8A, 80V, TO-220AC, Schottky Rect</t>
-  </si>
-  <si>
     <t>D2</t>
   </si>
   <si>
@@ -312,12 +306,6 @@
     <t>Price $</t>
   </si>
   <si>
-    <t>V5629G</t>
-  </si>
-  <si>
-    <t>TO-220F Heatsink</t>
-  </si>
-  <si>
     <t>HeatSink2</t>
   </si>
   <si>
@@ -330,9 +318,6 @@
     <t>TO-220 Heatsink</t>
   </si>
   <si>
-    <t>HeatSink3</t>
-  </si>
-  <si>
     <t>HSE-B1711-032</t>
   </si>
   <si>
@@ -343,6 +328,12 @@
   </si>
   <si>
     <t>Component Price</t>
+  </si>
+  <si>
+    <t>8TQ100</t>
+  </si>
+  <si>
+    <t>8A, 100V, TO-220AC, Schottky Rect</t>
   </si>
 </sst>
 </file>
@@ -765,7 +756,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,13 +777,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -897,16 +888,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -917,16 +908,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
@@ -937,16 +928,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
@@ -957,16 +948,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -977,16 +968,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -997,16 +988,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
@@ -1017,16 +1008,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="E13" s="3">
         <v>4</v>
@@ -1037,16 +1028,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="E14" s="3">
         <v>2</v>
@@ -1057,16 +1048,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
@@ -1077,16 +1068,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
@@ -1097,16 +1088,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
@@ -1117,16 +1108,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="E18" s="3">
         <v>1</v>
@@ -1137,16 +1128,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E19" s="3">
         <v>1</v>
@@ -1157,16 +1148,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="E20" s="3">
         <v>2</v>
@@ -1177,16 +1168,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
@@ -1197,16 +1188,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="E22" s="3">
         <v>1</v>
@@ -1217,16 +1208,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="E23" s="3">
         <v>1</v>
@@ -1237,16 +1228,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="D24" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E24" s="3">
         <v>1</v>
@@ -1256,33 +1247,23 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>94</v>
-      </c>
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="10"/>
-      <c r="D25" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E25" s="11">
-        <v>1</v>
-      </c>
-      <c r="F25" s="6">
-        <v>0.68</v>
-      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E26" s="11">
         <v>1</v>
@@ -1293,20 +1274,20 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E27" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="6">
-        <v>0.28000000000000003</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1314,11 +1295,11 @@
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="12" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F28" s="13">
         <f>SUM(F2:F27)</f>
-        <v>27.08</v>
+        <v>26.679999999999996</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1326,7 +1307,7 @@
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="12" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F29" s="12">
         <v>1.1299999999999999</v>
@@ -1337,11 +1318,11 @@
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F30" s="13">
         <f>SUM(F28:F29)</f>
-        <v>28.209999999999997</v>
+        <v>27.809999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>